<commit_message>
Add content owner detail report
</commit_message>
<xml_diff>
--- a/public/exports/ktv_report.xlsx
+++ b/public/exports/ktv_report.xlsx
@@ -38,28 +38,28 @@
     <t>Tổng tiền</t>
   </si>
   <si>
-    <t>Sơn Mi</t>
+    <t>Uông Cương</t>
   </si>
   <si>
     <t>Hồ Chí Minh</t>
   </si>
   <si>
-    <t>4, Thôn Giáp Hàn, Xã 09, Quận Ong Mi Thái Bình</t>
-  </si>
-  <si>
-    <t>84-231-385-7012</t>
-  </si>
-  <si>
-    <t>54.420.000 VNĐ</t>
-  </si>
-  <si>
-    <t>Cô. Tiêu Nghi Ánh</t>
-  </si>
-  <si>
-    <t>068-809-7276</t>
-  </si>
-  <si>
-    <t>55.960.000 VNĐ</t>
+    <t>1, Ấp An, Ấp Triệu Nguyệt, Quận Thiện Trà Vinh</t>
+  </si>
+  <si>
+    <t>(090)046-8046</t>
+  </si>
+  <si>
+    <t>3.392.800 VNĐ</t>
+  </si>
+  <si>
+    <t>Thịnh Khai Hiếu</t>
+  </si>
+  <si>
+    <t>(84)(96)555-5261</t>
+  </si>
+  <si>
+    <t>3.257.000 VNĐ</t>
   </si>
 </sst>
 </file>
@@ -423,9 +423,9 @@
     <col min="2" max="2" width="20.947266" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="13.877563" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="55.117493" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="18.590698" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="19.899902" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="26.838684" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="17.412415" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="16.234131" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -453,7 +453,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -468,7 +468,7 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>2721</v>
+        <v>16964</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -491,7 +491,7 @@
         <v>13</v>
       </c>
       <c r="F3">
-        <v>2798</v>
+        <v>16285</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>

</xml_diff>